<commit_message>
Update Direccionamiento Redes TFG.xlsx
</commit_message>
<xml_diff>
--- a/Lab/Direccionamiento Redes TFG.xlsx
+++ b/Lab/Direccionamiento Redes TFG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luist\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luist\Documents\GitHub\TFGCiscoDNA\Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0E9827-035F-4726-AF20-9DE0F1326E2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D84FB75A-9B7C-4A91-A22F-BA42CBDB4CBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="27">
   <si>
     <t>DISPOSITIVO</t>
   </si>
@@ -91,6 +91,21 @@
   </si>
   <si>
     <t>192.168.0.126</t>
+  </si>
+  <si>
+    <t>10.10.20.181</t>
+  </si>
+  <si>
+    <t>/24</t>
+  </si>
+  <si>
+    <t>10.10.20.182</t>
+  </si>
+  <si>
+    <t>10.10.20.183</t>
+  </si>
+  <si>
+    <t>GigabitEthernet5</t>
   </si>
 </sst>
 </file>
@@ -114,7 +129,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -127,8 +142,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -136,18 +157,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,168 +501,213 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="2"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E16" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>